<commit_message>
Fix Team name mismatches in data and few bits
Signed-off-by: Supun De Silva <supun1001@gmail.com>
</commit_message>
<xml_diff>
--- a/data_samples/afl-home-grounds.xlsx
+++ b/data_samples/afl-home-grounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ML101\data_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94AB88-80F6-4206-A679-7CE960DC1DB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AE2BF7-F54B-4234-B528-5AEA6A689358}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Geelong</t>
   </si>
   <si>
-    <t>Gold Coast Suns</t>
-  </si>
-  <si>
     <t>Carrara Stadium</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>MCG</t>
   </si>
   <si>
-    <t>North Melborne</t>
-  </si>
-  <si>
     <t>Melbourne</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>Name_in_Data</t>
+  </si>
+  <si>
+    <t>North Melbourne</t>
+  </si>
+  <si>
+    <t>Gold Coast</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,13 +465,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -551,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -567,68 +567,68 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
         <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -636,50 +636,50 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>